<commit_message>
Project requirements- translated. BugReport and SmokeTest- minor changes
</commit_message>
<xml_diff>
--- a/PetStoreBugReport.xlsx
+++ b/PetStoreBugReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usavrsavanje\IT BootCamp\Kurs\QA6\test_PetStore_ITBootCampProject\BugDoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usavrsavanje\IT BootCamp\Kurs\QA6\test_PetStore_ITBootCampProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92661F08-769C-4566-B365-CE8B81CE31F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EA14C4-466B-483B-B651-CE5D4EEB71B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,21 +136,12 @@
     <t>Registered user is able to make an order by just clicking on "Confirm" button, with prefilled and fake data.</t>
   </si>
   <si>
-    <t>Opens birds page when clicked on main manu central picture</t>
-  </si>
-  <si>
-    <t>a)Conclusion is drawn from the fact that when clicked on site logo in top left corner, the manu page is opened.                                                               b)On the other note, if the flagship item in PetStore are birds, than this might not be a bug, but an intentional.</t>
-  </si>
-  <si>
     <t>Manu page is reopened.</t>
   </si>
   <si>
     <t>Birds page is opened</t>
   </si>
   <si>
-    <t>When clicked on the central main picture of manu page, birds page is opened instead of reopening manu page.</t>
-  </si>
-  <si>
     <t>Help page; Stock</t>
   </si>
   <si>
@@ -160,16 +151,7 @@
     <t>Show "backordered" under "In Stock?" if the Quantity is higher, but completely unable the order to be submitted if the quantity is higher than JPetStore is able to manage.</t>
   </si>
   <si>
-    <t>"In Stock?" on Shopping Cart page doesn't show "backordered" if the Quanity is higher. Order is submitted for iregular quantities, which can not be managed.</t>
-  </si>
-  <si>
-    <t>It is posible to submit order for Quantities abnormally higher than in Stock. Under "In Stock?" on Shopping Cart page, it doesn't show "backordered" if Quanitity is higher than in stock.</t>
-  </si>
-  <si>
     <t>dev team</t>
-  </si>
-  <si>
-    <t>Contact client and ask for the manageable order qantity.</t>
   </si>
   <si>
     <t>Value4</t>
@@ -201,12 +183,6 @@
   </si>
   <si>
     <t>Value7</t>
-  </si>
-  <si>
-    <t>displayed unordered items list: Fish, Dogs, Reptiles, Cats, Birds, with dedicated discription</t>
-  </si>
-  <si>
-    <t>displayed unordered items list: Fish, Dogs, Cats, Reptiles,  Birds, with dedicated discription</t>
   </si>
   <si>
     <t>Same image is displayed for both Angelfish items</t>
@@ -484,37 +460,22 @@
     <t>Image of item breed "Golden Retriever"</t>
   </si>
   <si>
-    <t>Dulicate 1st and 3rd item description on "Labrador Retriever" product page</t>
-  </si>
-  <si>
     <t>1.Open Chrome browser; 2.input URL https://petstore.octoperf.com/ and click Enter key; 3. Click "Enter the Store"; Click on left menu category "Dogs"; Click on "Labrador Retriever" product ID</t>
   </si>
   <si>
     <t>Observe 1st and 3rd item description</t>
   </si>
   <si>
-    <t>Diferent items description</t>
-  </si>
-  <si>
     <t>Same items description</t>
   </si>
   <si>
-    <t>First and third item description are the same, where they shoud be different.</t>
-  </si>
-  <si>
     <t>Value21</t>
   </si>
   <si>
     <t>Value20</t>
   </si>
   <si>
-    <t>Dulicate 2nd and 4th item description on "Labrador Retriever" product page</t>
-  </si>
-  <si>
     <t>Check if some other more descriptive word should be included in 3rd item description, since prices and item IDs are different</t>
-  </si>
-  <si>
-    <t>Second and fourth item description are the same, where they shoud be different.</t>
   </si>
   <si>
     <t>Observe 2nd and 4th item description</t>
@@ -633,9 +594,6 @@
     <t>Value30</t>
   </si>
   <si>
-    <t>Category name "Cats" is not centered as other WebElements are</t>
-  </si>
-  <si>
     <t>1.Open Chrome browser; 2.input URL https://petstore.octoperf.com/ and click Enter key; 3. Click "Enter the Store"; Click on left menu category "Cats"</t>
   </si>
   <si>
@@ -643,15 +601,6 @@
 </t>
   </si>
   <si>
-    <t>Category name "Cats" is centered</t>
-  </si>
-  <si>
-    <t>Category name "Cats" is not centered</t>
-  </si>
-  <si>
-    <t>Category name "Cats" is not aligned and centered as other WebElements are</t>
-  </si>
-  <si>
     <t>Value31</t>
   </si>
   <si>
@@ -706,54 +655,18 @@
     <t>Value34</t>
   </si>
   <si>
-    <t>Category name "Reptiles" is not centered as other WebElements are</t>
-  </si>
-  <si>
     <t>1.Open Chrome browser; 2.input URL https://petstore.octoperf.com/ and click Enter key; 3. Click "Enter the Store"; Click on left menu category "Reptiles"</t>
   </si>
   <si>
-    <t>Category name "Reptiles" is centered</t>
-  </si>
-  <si>
-    <t>Category name "Reptiles" is not centered</t>
-  </si>
-  <si>
-    <t>Category name "Reptiles" is not aligned and centered as other WebElements are</t>
-  </si>
-  <si>
-    <t>Category name "Dogs" is not centered as other WebElements are</t>
-  </si>
-  <si>
     <t>1.Open Chrome browser; 2.input URL https://petstore.octoperf.com/ and click Enter key; 3. Click "Enter the Store"; Click on left menu category "Dogs"</t>
   </si>
   <si>
-    <t>Category name "Dogs" is centered</t>
-  </si>
-  <si>
-    <t>Category name "Dogs" is not centered</t>
-  </si>
-  <si>
-    <t>Category name "Dogs" is not aligned and centered as other WebElements are</t>
-  </si>
-  <si>
     <t>Wrong order in left item list on menu page</t>
   </si>
   <si>
-    <t>Category name "Fish" is not centered as other WebElements are</t>
-  </si>
-  <si>
     <t>1.Open Chrome browser; 2.input URL https://petstore.octoperf.com/ and click Enter key; 3. Click "Enter the Store"; Click on left menu category "Fish"</t>
   </si>
   <si>
-    <t>Category name "Fish" is centered</t>
-  </si>
-  <si>
-    <t>Category name "Fish" is not centered</t>
-  </si>
-  <si>
-    <t>Category name "Fish" is not aligned and centered as other WebElements are</t>
-  </si>
-  <si>
     <t>Same image for both "Rattlesnake" items</t>
   </si>
   <si>
@@ -773,9 +686,6 @@
   </si>
   <si>
     <t>Description of item with " Venomless" word</t>
-  </si>
-  <si>
-    <t>Becouse of the fact that there are no venomless Rattlesnakes, word "venomless" is not needed</t>
   </si>
   <si>
     <t>Non existing species "Venomless Rattlesnake" on item page</t>
@@ -808,19 +718,7 @@
     <t>There are only 2 products "Lizards" and "Snakes", and no "Turtles"</t>
   </si>
   <si>
-    <t>Category name "Birds" is not centered as other WebElements are</t>
-  </si>
-  <si>
     <t>1.Open Chrome browser; 2.input URL https://petstore.octoperf.com/ and click Enter key; 3. Click "Enter the Store"; Click on left menu category "Birds"</t>
-  </si>
-  <si>
-    <t>Category name "Birds" is centered</t>
-  </si>
-  <si>
-    <t>Category name "Birds" is not centered</t>
-  </si>
-  <si>
-    <t>Category name "Birds" is not aligned and centered as other WebElements are</t>
   </si>
   <si>
     <t>Summery note: - All images should be checked again with the client.
@@ -895,15 +793,6 @@
 15.Observe that there is no items in the shopping cart</t>
   </si>
   <si>
-    <t>Items added to shopping cart should remain in shopping cart after user has loged out</t>
-  </si>
-  <si>
-    <t>Items added to shopping cart did not remain in shopping cart after user has loged out</t>
-  </si>
-  <si>
-    <t>After adding items in shopping cart and loging out, user has to add items of interest in the shopping cart once again because they are no longer there</t>
-  </si>
-  <si>
     <t>Boolean values for  "In Stock?" item status in Shopping Cart</t>
   </si>
   <si>
@@ -919,9 +808,6 @@
   </si>
   <si>
     <t>If the item is not in stock it should show "backordered" and not false, according to the Help page documentation</t>
-  </si>
-  <si>
-    <t>When the user chooses to buy items which are not in stock and goes to Shopping Cart, "In Stock?" status should state "backordered" and not boolean values true/false</t>
   </si>
   <si>
     <t>Value45</t>
@@ -957,9 +843,6 @@
     <t>The user is able to remove only 1 item from the Shopping Cart and if he tries to remove another one, the duplicate message "Attempted to remove null CartItem from Cart." is  displayed</t>
   </si>
   <si>
-    <t>User can remove only 1 item from Shoppin Cart</t>
-  </si>
-  <si>
     <t>Value47</t>
   </si>
   <si>
@@ -995,12 +878,6 @@
     <t>There is no clickable JPetStore text or Logo for the user to go back on the Manu page</t>
   </si>
   <si>
-    <t>Clickable text or Logo so the user could easaly go back to shopping</t>
-  </si>
-  <si>
-    <t>clickable text or Logo so the user could easaly go back to shopping doesn't exist</t>
-  </si>
-  <si>
     <t>User is not able to intuitively go back to shopping by clicking on clickable Logo of the JPetStore</t>
   </si>
   <si>
@@ -1020,15 +897,6 @@
 </t>
   </si>
   <si>
-    <t>Search field is in the center of the banner</t>
-  </si>
-  <si>
-    <t>Search field is in the center of the banner is in the right corner of the banner</t>
-  </si>
-  <si>
-    <t>Search filed and Help page instructions do not match. Search filed is on the right, instead in the center.</t>
-  </si>
-  <si>
     <t>Value49</t>
   </si>
   <si>
@@ -1038,14 +906,6 @@
     <t>Search input "Tiger Shark" displays two items</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1.Click on sarch filed
-2.Type "Tiger Shark"
-3. Click search button
-4.Observe search results
-</t>
-  </si>
-  <si>
     <t>Only one item is displayed</t>
   </si>
   <si>
@@ -1055,14 +915,6 @@
     <t>Value51</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1.Click on sarch filed
-2.Type "Golden Retriever"
-3. Click search button
-4.Observe search results
-</t>
-  </si>
-  <si>
     <t>Two same items and one wrong, are displayed</t>
   </si>
   <si>
@@ -1075,28 +927,12 @@
     <t>Search input "Lab Retriever" displays 2 duplicate items and 1 wrong</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1.Click on sarch filed
-2.Type "Lab Retriever"
-3. Click search button
-4.Observe search results
-</t>
-  </si>
-  <si>
     <t>Value53</t>
   </si>
   <si>
     <t>Search input "Amazon Parrot" displays 2 duplicate items</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1.Click on sarch filed
-2.Type "Amazon Parrot"
-3. Click search button
-4.Observe search results
-</t>
-  </si>
-  <si>
     <t>When user inputs exact name of the product, there should be no duplicates or wrong search results</t>
   </si>
   <si>
@@ -1112,14 +948,6 @@
     <t>Search input "parot" displays no items</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1.Click on sarch filed
-2.Type "parot"
-3. Click search button
-4.Observe search results
-</t>
-  </si>
-  <si>
     <t>No items are in search results</t>
   </si>
   <si>
@@ -1130,9 +958,6 @@
   </si>
   <si>
     <t>Value55</t>
-  </si>
-  <si>
-    <t>Preinput text in password field on Sign in</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1146,27 +971,7 @@
     <t>Password field is empty has text</t>
   </si>
   <si>
-    <t xml:space="preserve">When user tries to log in the password filed is allready filled </t>
-  </si>
-  <si>
-    <t>My Account information password is not encripted on input</t>
-  </si>
-  <si>
     <t>Value56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1.Click on Sign in clickable text
-2. Click on password field
-3. Input "jo123"
-4. Repat same input in field bellow 
-5.Observe password and repeated password field</t>
-  </si>
-  <si>
-    <t>Password text should be encripted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password text is not encripted </t>
   </si>
   <si>
     <t>Value57</t>
@@ -1181,9 +986,6 @@
   </si>
   <si>
     <t>My Account information "First name:" is not saved after logout</t>
-  </si>
-  <si>
-    <t>Other fileds should be checked too.</t>
   </si>
   <si>
     <t>When user enters new password and repeats it bellow, the password text is not encrypted</t>
@@ -1231,10 +1033,208 @@
     <t>User is registered with fake data</t>
   </si>
   <si>
-    <t>User is enabled to input fake data in registaration fields and to register</t>
-  </si>
-  <si>
-    <t>a)Conclusion is drawn from the fact that top and central items lists on manu page are the same.</t>
+    <t xml:space="preserve">
+1.Click on search filed
+2.Type "Tiger Shark"
+3. Click search button
+4.Observe search results
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Click on search filed
+2.Type "Golden Retriever"
+3. Click search button
+4.Observe search results
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Click on search filed
+2.Type "Lab Retriever"
+3. Click search button
+4.Observe search results
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Click on search filed
+2.Type "Amazon Parrot"
+3. Click search button
+4.Observe search results
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Click on search filed
+2.Type "parot"
+3. Click search button
+4.Observe search results
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Click on Sign in clickable text
+2. Click on password field
+3. Input "jo123"
+4. Repeat same input in field bellow 
+5.Observe password and repeated password field</t>
+  </si>
+  <si>
+    <t>displayed unordered items list: Fish, Dogs, Reptiles, Cats, Birds, with dedicated description</t>
+  </si>
+  <si>
+    <t>Category name "Fish" is centred</t>
+  </si>
+  <si>
+    <t>Category name "Dogs" is centred</t>
+  </si>
+  <si>
+    <t>Different items description</t>
+  </si>
+  <si>
+    <t>Category name "Cats" is centred</t>
+  </si>
+  <si>
+    <t>Category name "Reptiles" is centred</t>
+  </si>
+  <si>
+    <t>Category name "Birds" is centred</t>
+  </si>
+  <si>
+    <t>Items added to shopping cart should remain in shopping cart after user has logged out</t>
+  </si>
+  <si>
+    <t>Clickable text or Logo so the user could easily go back to shopping</t>
+  </si>
+  <si>
+    <t>Search field is in the centre of the banner</t>
+  </si>
+  <si>
+    <t>Password text should be encrypted</t>
+  </si>
+  <si>
+    <t>"In Stock?" on Shopping Cart page doesn't show "backordered" if the Quantity is higher. Order is submitted for irregular quantities, which can not be managed.</t>
+  </si>
+  <si>
+    <t>displayed unordered items list: Fish, Dogs, Cats, Reptiles,  Birds, with dedicated description</t>
+  </si>
+  <si>
+    <t>Category name "Fish" is not centred</t>
+  </si>
+  <si>
+    <t>Category name "Dogs" is not centred</t>
+  </si>
+  <si>
+    <t>Category name "Cats" is not centred</t>
+  </si>
+  <si>
+    <t>Category name "Reptiles" is not centred</t>
+  </si>
+  <si>
+    <t>Category name "Birds" is not centred</t>
+  </si>
+  <si>
+    <t>Items added to shopping cart did not remain in shopping cart after user has logged out</t>
+  </si>
+  <si>
+    <t>clickable text or Logo so the user could easily go back to shopping doesn't exist</t>
+  </si>
+  <si>
+    <t>Search field is in the centre of the banner is in the right corner of the banner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password text is not encrypted </t>
+  </si>
+  <si>
+    <t>It is possible to submit order for Quantities abnormally higher than in Stock. Under "In Stock?" on Shopping Cart page, it doesn't show "backordered" if Quantity is higher than in stock.</t>
+  </si>
+  <si>
+    <t>When clicked on the central main picture of menu page, birds page is opened instead of reopening menu page.</t>
+  </si>
+  <si>
+    <t>Category name "Fish" is not aligned and centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Category name "Dogs" is not aligned and centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>First and third item description are the same, where they should be different.</t>
+  </si>
+  <si>
+    <t>Second and fourth item description are the same, where they should be different.</t>
+  </si>
+  <si>
+    <t>Category name "Cats" is not aligned and centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Category name "Reptiles" is not aligned and centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Because of the fact that there are no venomless Rattlesnakes, word "venomless" is not needed</t>
+  </si>
+  <si>
+    <t>Category name "Birds" is not aligned and centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>After adding items in shopping cart and logging out, user has to add items of interest in the shopping cart once again because they are no longer there</t>
+  </si>
+  <si>
+    <t>When the user chooses to buy items which are not in stock and goes to Shopping Cart, "In Stock?" status should state "backordered" and not Boolean values true/false</t>
+  </si>
+  <si>
+    <t>Search filed and Help page instructions do not match. Search filed is on the right, instead in the centre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user tries to log in the password filed is already filled </t>
+  </si>
+  <si>
+    <t>User is enabled to input fake data in registration fields and to register</t>
+  </si>
+  <si>
+    <t>Contact client and ask for the manageable order quantity.</t>
+  </si>
+  <si>
+    <t>a)Conclusion is drawn from the fact that when clicked on site logo in top left corner, the menu page is opened.                                                               b)On the other note, if the flagship item in PetStore are birds, than this might not be a bug, but an intentional.</t>
+  </si>
+  <si>
+    <t>a)Conclusion is drawn from the fact that top and central items lists on menu page are the same.</t>
+  </si>
+  <si>
+    <t>Other fields should be checked too.</t>
+  </si>
+  <si>
+    <t>Opens birds page when clicked on main menu central picture</t>
+  </si>
+  <si>
+    <t>Category name "Fish" is not centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Category name "Dogs" is not centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Duplicated 1st and 3rd item description on "Labrador Retriever" product page</t>
+  </si>
+  <si>
+    <t>Duplicated 2nd and 4th item description on "Labrador Retriever" product page</t>
+  </si>
+  <si>
+    <t>Category name "Cats" is not centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Category name "Reptiles" is not centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>Category name "Birds" is not centred as other WebElements are</t>
+  </si>
+  <si>
+    <t>User can remove only 1 item from Shopping Cart</t>
+  </si>
+  <si>
+    <t>My Account information password is not encrypted on input</t>
+  </si>
+  <si>
+    <t>Text in password field on Sign in</t>
   </si>
 </sst>
 </file>
@@ -5971,7 +5971,7 @@
   <dimension ref="A1:BH21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
@@ -6007,169 +6007,169 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="AK1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="AS1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="AV1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="BF1" s="1" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>346</v>
+        <v>291</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>354</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:60" ht="15.75">
@@ -6363,175 +6363,175 @@
         <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>351</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>233</v>
+        <v>352</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="AS3" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="AP3" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AT3" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="AW3" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="BB3" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="BC3" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="BD3" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="AV3" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX3" s="3" t="s">
+      <c r="BE3" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="BF3" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="BG3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BH3" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="AZ3" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="BA3" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="BB3" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="BC3" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="BD3" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="BE3" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="BF3" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="BG3" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="BH3" s="3" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:60" ht="15.75">
@@ -6729,169 +6729,169 @@
         <v>33</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AG5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AK5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AM5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AN5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AO5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AP5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AQ5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AR5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AS5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AT5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="AU5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="AV5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="AW5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="AX5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="AY5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="AZ5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BA5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BB5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BC5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BD5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BE5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BF5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BG5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="BH5" s="3" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:60" ht="15.75">
@@ -6903,7 +6903,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -7062,10 +7062,10 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
       <c r="AE8" s="3" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="AF8" s="3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
@@ -7461,175 +7461,175 @@
         <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="K11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="AK11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AM11" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AP11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AQ11" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AR11" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AS11" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AB11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG11" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH11" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AI11" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="AK11" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="AL11" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="AM11" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AN11" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="AO11" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="AP11" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="AQ11" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="AR11" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AS11" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="AT11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="AU11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="AV11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="AW11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="AX11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="AY11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="AZ11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BA11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BB11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BC11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BD11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BE11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BF11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BG11" s="3" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="BH11" s="3" t="s">
-        <v>355</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:60" ht="216.75">
@@ -7638,178 +7638,178 @@
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="AD12" s="3" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="AE12" s="3" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="AF12" s="3" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="AG12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AK12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AL12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AM12" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="AO12" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="AP12" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="AQ12" s="3" t="s">
-        <v>251</v>
+        <v>221</v>
       </c>
       <c r="AR12" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="AS12" s="3" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="AT12" s="3" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="AU12" s="3" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="AV12" s="3" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="AW12" s="3" t="s">
-        <v>295</v>
+        <v>256</v>
       </c>
       <c r="AX12" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="AY12" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AZ12" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="BA12" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="AY12" s="3" t="s">
+      <c r="BB12" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="AZ12" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="BA12" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB12" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="BC12" s="3" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="BD12" s="3" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="BE12" s="3" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="BF12" s="3" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
       <c r="BG12" s="3" t="s">
-        <v>347</v>
+        <v>292</v>
       </c>
       <c r="BH12" s="3" t="s">
-        <v>357</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:60" ht="51">
@@ -7821,175 +7821,175 @@
         <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>60</v>
+        <v>310</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>235</v>
+        <v>311</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG13" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH13" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI13" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AK13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AL13" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AM13" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="AN13" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="AO13" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP13" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="AQ13" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="AR13" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AS13" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AC13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AD13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AG13" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH13" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="AI13" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="AJ13" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="AK13" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="AL13" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="AM13" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="AN13" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="AO13" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="AP13" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="AQ13" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="AR13" s="3" t="s">
+      <c r="AT13" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="AU13" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="AV13" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="AW13" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="AS13" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="AT13" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="AU13" s="3" t="s">
+      <c r="AX13" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="AY13" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AZ13" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="BA13" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB13" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="BC13" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="BD13" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="AV13" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="AW13" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="AX13" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="AY13" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="AZ13" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="BA13" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="BB13" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="BC13" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="BD13" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="BE13" s="3" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="BF13" s="3" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="BG13" s="3" t="s">
-        <v>351</v>
+        <v>295</v>
       </c>
       <c r="BH13" s="3" t="s">
-        <v>358</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:60" ht="51">
@@ -8001,175 +8001,175 @@
         <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>46</v>
+        <v>321</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>236</v>
+        <v>323</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH14" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI14" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AK14" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AL14" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AM14" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="AN14" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AO14" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AP14" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AQ14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="AR14" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="AS14" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AE14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG14" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="AH14" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="AI14" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="AK14" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AL14" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AM14" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AN14" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="AO14" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AP14" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="AQ14" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="AR14" s="3" t="s">
+      <c r="AT14" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AU14" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AV14" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AW14" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="AS14" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="AT14" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="AU14" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="AV14" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="AW14" s="3" t="s">
-        <v>297</v>
-      </c>
       <c r="AX14" s="3" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="AY14" s="3" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="AZ14" s="3" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="BA14" s="3" t="s">
-        <v>318</v>
+        <v>272</v>
       </c>
       <c r="BB14" s="3" t="s">
-        <v>318</v>
+        <v>272</v>
       </c>
       <c r="BC14" s="3" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="BD14" s="3" t="s">
-        <v>332</v>
+        <v>283</v>
       </c>
       <c r="BE14" s="3" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="BF14" s="3" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="BG14" s="3" t="s">
-        <v>352</v>
+        <v>296</v>
       </c>
       <c r="BH14" s="3" t="s">
-        <v>359</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:60" ht="60.75" customHeight="1">
@@ -8181,175 +8181,175 @@
         <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>237</v>
+        <v>334</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L15" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AG15" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH15" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI15" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK15" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AL15" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AM15" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="AN15" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AO15" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="AP15" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="AQ15" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AR15" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="AS15" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z15" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AB15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AC15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AD15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AG15" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH15" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AI15" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AJ15" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AK15" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="AL15" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AM15" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="AN15" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="AO15" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="AP15" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="AQ15" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AR15" s="3" t="s">
+      <c r="AT15" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU15" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="AV15" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AW15" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="AS15" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="AT15" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="AU15" s="3" t="s">
+      <c r="AX15" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="AY15" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="AZ15" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="BA15" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="BB15" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="BC15" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="BD15" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AV15" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="AW15" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="AX15" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="AY15" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="AZ15" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="BA15" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="BB15" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="BC15" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="BD15" s="3" t="s">
-        <v>334</v>
-      </c>
       <c r="BE15" s="3" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="BF15" s="3" t="s">
-        <v>350</v>
+        <v>294</v>
       </c>
       <c r="BG15" s="3" t="s">
-        <v>353</v>
+        <v>297</v>
       </c>
       <c r="BH15" s="3" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:60" ht="15.75">
@@ -8366,157 +8366,157 @@
         <v>30</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="X16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AC16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AD16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AE16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AI16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AJ16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AK16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AL16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AM16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AN16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AO16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AP16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AQ16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AR16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AS16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AT16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AU16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AV16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="AW16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AX16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AY16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AZ16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BA16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BB16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BC16" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BD16" s="3" t="s">
         <v>27</v>
@@ -8540,178 +8540,178 @@
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="X17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AA17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AD17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AE17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AG17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AH17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AI17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AJ17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AK17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AL17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AM17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AN17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AO17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AP17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AQ17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AR17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AS17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AT17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AU17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AV17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AW17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AX17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AY17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AZ17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BA17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BB17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BC17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BD17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BE17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BF17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BG17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="BH17" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:60" ht="15.75">
@@ -8726,127 +8726,127 @@
         <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AD18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AG18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AH18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AI18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AJ18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AK18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AL18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AM18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AN18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AO18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AP18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AQ18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AR18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AS18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AT18" s="3" t="s">
         <v>27</v>
@@ -8855,34 +8855,34 @@
         <v>27</v>
       </c>
       <c r="AV18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AW18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AX18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AY18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AZ18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BA18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BB18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BC18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BD18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BE18" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="BF18" s="3" t="s">
         <v>30</v>
@@ -8903,42 +8903,42 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>347</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>348</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -8947,45 +8947,45 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="Z19" s="3" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="AA19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AB19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AD19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AE19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AF19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AG19" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="AH19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="AK19" s="3"/>
       <c r="AL19" s="3" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="AM19" s="3"/>
       <c r="AN19" s="3"/>
@@ -8994,7 +8994,7 @@
       <c r="AQ19" s="3"/>
       <c r="AR19" s="3"/>
       <c r="AS19" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="AT19" s="3"/>
       <c r="AU19" s="3"/>
@@ -9010,15 +9010,15 @@
       <c r="BE19" s="3"/>
       <c r="BF19" s="3"/>
       <c r="BG19" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="BH19" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:60" ht="154.5" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>